<commit_message>
mals2-19 add column to report
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453E524-537E-4737-9AE7-160183E24278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="7695" yWindow="4335" windowWidth="30195" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].Penalty}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +550,7 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +564,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -573,7 +580,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +589,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +616,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +629,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +656,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +670,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -689,6 +704,7 @@
       <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="I11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -700,12 +716,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -932,15 +945,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -965,18 +990,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #477 from bcgov/MALS2-17-18-19-24"
This reverts commit 30185cd52166ba10095664a5d73e859bb229b87b, reversing
changes made to fbe1335acba21a1b6b7767c5a991ec5469a817e1.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453E524-537E-4737-9AE7-160183E24278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7695" yWindow="4335" windowWidth="30195" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Client</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
-  </si>
-  <si>
-    <t>Penalty Issued</t>
-  </si>
-  <si>
-    <t>{d.Reg[i].Penalty}</t>
   </si>
 </sst>
 </file>
@@ -178,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -217,7 +211,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -236,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -382,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -532,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +543,7 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -564,7 +557,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -580,7 +573,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -589,9 +582,8 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -616,11 +608,8 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -629,9 +618,8 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -656,11 +644,8 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -670,22 +655,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -704,7 +689,6 @@
       <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -716,9 +700,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -945,27 +932,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -990,9 +965,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reapply "Merge pull request #477 from bcgov/MALS2-17-18-19-24"
This reverts commit e4fa36c9a47e507cdd299ed55467ccbd0a5f3168.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2453E524-537E-4737-9AE7-160183E24278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="7695" yWindow="4335" windowWidth="30195" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].Penalty}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,6 +217,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +550,7 @@
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +564,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -573,7 +580,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +589,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +616,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +629,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +656,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +670,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -689,6 +704,7 @@
       <c r="H11" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="I11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -700,12 +716,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -932,15 +945,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -965,18 +990,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add 5.5 changes back in
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,6 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,9 +548,10 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +565,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -570,10 +578,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +590,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +630,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +657,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +671,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,15 +716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -931,21 +938,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -964,7 +972,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -979,4 +987,12 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #490 from bcgov/bf-revert-5.5-2"
This reverts commit d28dd6b98b9c1d9c84f7d42e8645fbf1594d1b84, reversing
changes made to 3ab5d9c80c57fa083252d021ff2ce60e5e23f4e4.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,6 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,9 +548,10 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +565,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -570,10 +578,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +590,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +630,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +657,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +671,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,15 +716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -931,21 +938,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -964,7 +972,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -979,4 +987,12 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #491 from bcgov/reapply-5.5-2"
This reverts commit d2937a9fc4c57dabb4a0a3d4115024e86b3fc4fe, reversing
changes made to d28dd6b98b9c1d9c84f7d42e8645fbf1594d1b84.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Client</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
-  </si>
-  <si>
-    <t>Penalty Issued</t>
-  </si>
-  <si>
-    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -178,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,7 +208,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -236,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -382,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -532,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +541,9 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -565,7 +557,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -578,10 +570,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -590,9 +582,8 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -617,11 +608,8 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -630,9 +618,8 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -657,11 +644,8 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -671,22 +655,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -716,6 +700,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -938,22 +931,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -972,7 +964,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -987,12 +979,4 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Merge pull request #493 from bcgov/revert-5.5-again"
This reverts commit bb48ff6a98c2af0f99c52028f14b2d5c2209158c, reversing
changes made to d2937a9fc4c57dabb4a0a3d4115024e86b3fc4fe.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,6 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,9 +548,10 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +565,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -570,10 +578,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +590,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +630,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +657,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +671,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,15 +716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -931,21 +938,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -964,7 +972,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -979,4 +987,12 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Reapply "Merge pull request #493 from bcgov/revert-5.5-again"
This reverts commit fdba444452404a67188ce470a6e310c054705e48.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Client</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
-  </si>
-  <si>
-    <t>Penalty Issued</t>
-  </si>
-  <si>
-    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -178,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,7 +208,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -236,9 +229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -276,7 +269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -382,7 +375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -532,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +541,9 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -565,7 +557,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -578,10 +570,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -590,9 +582,8 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -617,11 +608,8 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -630,9 +618,8 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -657,11 +644,8 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -671,22 +655,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -716,6 +700,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -938,22 +931,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -972,7 +964,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -987,12 +979,4 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Revert "Reapply "Merge pull request #493 from bcgov/revert-5.5-again""
This reverts commit 4e43d9529314bb045f9011868c5f5395aedf00cf.
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
+++ b/app/server/static/templates/reports/Dairy_Test_Threshold_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360457C1-2C74-4411-82E8-CF7BC12383F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B7213E-3B24-4304-B368-7A7A03999F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Threshold Report" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Client</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>Penalty Issued</t>
+  </si>
+  <si>
+    <t>{d.Reg[i].PenaltyIssued}</t>
   </si>
 </sst>
 </file>
@@ -172,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,6 +214,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -229,9 +236,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -269,7 +276,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -375,7 +382,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -517,7 +524,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -525,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,9 +548,10 @@
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>6</v>
       </c>
@@ -557,7 +565,7 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -570,10 +578,10 @@
       <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -582,8 +590,9 @@
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="I3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,8 +617,11 @@
       <c r="H4" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -618,8 +630,9 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="15"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -644,8 +657,11 @@
       <c r="H6" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -655,22 +671,22 @@
       </c>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="D8" s="9"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="D9" s="9"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="D10" s="9"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -700,15 +716,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0f00dee740a70860da74dc5110d51704">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2351f42212ae562663f11aa838f8e3a4" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -931,21 +938,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DAC4DD0-6527-4C33-8A5D-F6D18A2872ED}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -964,7 +972,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{028A420A-B050-4A61-806A-8D9C587E3D76}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -979,4 +987,12 @@
     <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F54B38D-A965-4592-A05D-BAAD7EF0EFBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>